<commit_message>
Update tests and tests data
</commit_message>
<xml_diff>
--- a/tests/domain/route_points/defect_010362.xlsx
+++ b/tests/domain/route_points/defect_010362.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hazin\Projects\bm-route-events\tests\domain\route_points\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6E90C3-6658-48DD-A6C4-B6F83A587249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8937BD-0844-4692-8902-B0F9DB708AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2550" windowWidth="29040" windowHeight="15720" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="1920" windowWidth="16800" windowHeight="9680" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="5" r:id="rId1"/>
@@ -1056,7 +1056,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A5"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1149,10 +1149,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="3">
-        <v>-6.8726482999999998</v>
+        <v>97.847362500000003</v>
       </c>
       <c r="D2" s="3">
-        <v>108.88429499999999</v>
+        <v>2.8316146</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>19</v>
@@ -1206,10 +1206,10 @@
         <v>10</v>
       </c>
       <c r="C3" s="3">
-        <v>-6.8726482000000004</v>
+        <v>97.847362500000003</v>
       </c>
       <c r="D3" s="3">
-        <v>108.88429499999999</v>
+        <v>2.8316146</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>19</v>
@@ -1263,10 +1263,10 @@
         <v>10</v>
       </c>
       <c r="C4" s="3">
-        <v>-6.8726481000000001</v>
+        <v>97.847362500000003</v>
       </c>
       <c r="D4" s="3">
-        <v>108.88429499999999</v>
+        <v>2.8316146</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
@@ -1320,10 +1320,10 @@
         <v>10</v>
       </c>
       <c r="C5" s="3">
-        <v>-6.8726478999999996</v>
+        <v>97.847362500000003</v>
       </c>
       <c r="D5" s="3">
-        <v>108.88429499999999</v>
+        <v>2.8316146</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Update test and test data
</commit_message>
<xml_diff>
--- a/tests/domain/route_points/defect_010362.xlsx
+++ b/tests/domain/route_points/defect_010362.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hazin\Projects\bm-route-events\tests\domain\route_points\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8937BD-0844-4692-8902-B0F9DB708AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1917EFA7-3C8E-4661-B4A9-18D0286C0507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1920" windowWidth="16800" windowHeight="9680" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
   <si>
     <t>linkid</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>010362</t>
+  </si>
+  <si>
+    <t>21</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1059,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1275,7 +1278,7 @@
         <v>29</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8" t="s">
@@ -1332,7 +1335,7 @@
         <v>31</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8" t="s">

</xml_diff>

<commit_message>
Add tests and change tests data
</commit_message>
<xml_diff>
--- a/tests/domain/route_points/defect_010362.xlsx
+++ b/tests/domain/route_points/defect_010362.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hazin\Projects\bm-route-events\tests\domain\route_points\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1917EFA7-3C8E-4661-B4A9-18D0286C0507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DF57F2-6330-4398-B21F-C97C718C9A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>linkid</t>
   </si>
@@ -66,15 +66,6 @@
     <t>defects_type</t>
   </si>
   <si>
-    <t>defects_width</t>
-  </si>
-  <si>
-    <t>defects_length</t>
-  </si>
-  <si>
-    <t>defects_vol</t>
-  </si>
-  <si>
     <t>defects_severity</t>
   </si>
   <si>
@@ -138,13 +129,16 @@
     <t>1</t>
   </si>
   <si>
-    <t>as_ravelling</t>
-  </si>
-  <si>
     <t>010362</t>
   </si>
   <si>
     <t>21</t>
+  </si>
+  <si>
+    <t>defects_dimension</t>
+  </si>
+  <si>
+    <t>as_raveling</t>
   </si>
 </sst>
 </file>
@@ -1053,13 +1047,13 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1073,19 +1067,17 @@
     <col min="7" max="7" width="10.1796875" style="15" customWidth="1"/>
     <col min="8" max="9" width="17" style="1"/>
     <col min="10" max="10" width="17.453125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="12.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="17" style="1"/>
+    <col min="11" max="11" width="16.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="17" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1117,36 +1109,30 @@
         <v>9</v>
       </c>
       <c r="K1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3">
         <v>10</v>
@@ -1158,52 +1144,46 @@
         <v>2.8316146</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="4">
+        <v>20</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>25</v>
+      <c r="N2" s="5">
+        <v>2018</v>
+      </c>
+      <c r="O2" s="5">
+        <v>1</v>
       </c>
       <c r="P2" s="5">
-        <v>2018</v>
+        <v>1</v>
       </c>
       <c r="Q2" s="5">
         <v>1</v>
       </c>
-      <c r="R2" s="5">
-        <v>1</v>
-      </c>
-      <c r="S2" s="5">
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3">
         <v>10</v>
@@ -1215,52 +1195,46 @@
         <v>2.8316146</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="4">
+        <v>20</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>25</v>
+      <c r="N3" s="5">
+        <v>2018</v>
+      </c>
+      <c r="O3" s="5">
+        <v>1</v>
       </c>
       <c r="P3" s="5">
-        <v>2018</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="5">
         <v>1</v>
       </c>
-      <c r="R3" s="5">
-        <v>1</v>
-      </c>
-      <c r="S3" s="5">
-        <v>1</v>
-      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3">
         <v>10</v>
@@ -1272,52 +1246,46 @@
         <v>2.8316146</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>25</v>
+      <c r="K4" s="4">
+        <v>20</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="5">
+        <v>2018</v>
+      </c>
+      <c r="O4" s="5">
+        <v>1</v>
       </c>
       <c r="P4" s="5">
-        <v>2018</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="5">
         <v>1</v>
       </c>
-      <c r="R4" s="5">
-        <v>1</v>
-      </c>
-      <c r="S4" s="5">
-        <v>1</v>
-      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3">
         <v>10</v>
@@ -1329,54 +1297,46 @@
         <v>2.8316146</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="4">
+        <v>20</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M5" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>25</v>
+      <c r="N5" s="5">
+        <v>2018</v>
+      </c>
+      <c r="O5" s="5">
+        <v>1</v>
       </c>
       <c r="P5" s="5">
-        <v>2018</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="5">
         <v>1</v>
       </c>
-      <c r="R5" s="5">
-        <v>1</v>
-      </c>
-      <c r="S5" s="5">
-        <v>1</v>
-      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>

</xml_diff>